<commit_message>
Connor: Finished updating evaluation/experimentation and updated conclusion of Dissertation.docx
</commit_message>
<xml_diff>
--- a/Documentation/Experiments/MachineLearningApplication.xlsx
+++ b/Documentation/Experiments/MachineLearningApplication.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="20">
   <si>
     <t>Iteration</t>
   </si>
@@ -74,6 +74,12 @@
   <si>
     <t>1,000 movies on edge</t>
   </si>
+  <si>
+    <t>Increase in time from 1,000 to 10,000</t>
+  </si>
+  <si>
+    <t>Decrease in Eclid dist from 1,000 to 10,000</t>
+  </si>
 </sst>
 </file>
 
@@ -116,7 +122,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -145,6 +151,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2099,6 +2108,822 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Request time</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="3"/>
+              <c:pt idx="0">
+                <c:v>1,000</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>10,000</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>100,000</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>('Basic Word Bank'!$B$29,'Basic Word Bank'!$F$29,'Basic Word Bank'!$J$29)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.23830000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.1284000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10.028200000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-094A-4F2C-AC24-D6E6F5BAD33E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1087535408"/>
+        <c:axId val="1195913776"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1087535408"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Number of movies on edge node</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1195913776"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1195913776"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Request</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> Time (s)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1087535408"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Euclidean</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" baseline="0"/>
+              <a:t> distance</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="3"/>
+              <c:pt idx="0">
+                <c:v>1,000</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>10,000</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>100,000</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>('Basic Word Bank'!$D$29,'Basic Word Bank'!$H$29,'Basic Word Bank'!$L$29)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.54243667725213007</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.39100890107911696</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.27847599394901595</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-037B-4006-9A4F-6E32ADA9AE96}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1087535408"/>
+        <c:axId val="1195913776"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1087535408"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="t"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Number of movies on edge node</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1195913776"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1195913776"/>
+        <c:scaling>
+          <c:orientation val="maxMin"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Euclidian Distance</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1087535408"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -2259,6 +3084,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -3918,6 +4823,1038 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -4319,7 +6256,7 @@
     <xdr:to>
       <xdr:col>35</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:row>40</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -4349,13 +6286,13 @@
     <xdr:from>
       <xdr:col>28</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>32</xdr:row>
+      <xdr:row>41</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>35</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>46</xdr:row>
+      <xdr:row>55</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -4385,13 +6322,13 @@
     <xdr:from>
       <xdr:col>28</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>47</xdr:row>
+      <xdr:row>56</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>35</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>62</xdr:row>
+      <xdr:row>71</xdr:row>
       <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -4412,6 +6349,80 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>5953</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>8334</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>82153</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>84534</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A86B50FA-F2F7-4EB7-8E01-AF752D0F9B18}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2C4F17E0-F7FE-4681-8C33-0527326C1003}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -4717,10 +6728,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AI94"/>
+  <dimension ref="A1:AI103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N19" sqref="N19:P28"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J37" sqref="J37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4844,29 +6855,29 @@
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
       <c r="E6" s="7"/>
-      <c r="F6" s="11" t="s">
+      <c r="F6" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="12"/>
       <c r="I6" s="8"/>
-      <c r="J6" s="11" t="s">
+      <c r="J6" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="K6" s="11"/>
-      <c r="L6" s="11"/>
+      <c r="K6" s="12"/>
+      <c r="L6" s="12"/>
       <c r="M6" s="8"/>
-      <c r="N6" s="11" t="s">
+      <c r="N6" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="O6" s="11"/>
-      <c r="P6" s="11"/>
+      <c r="O6" s="12"/>
+      <c r="P6" s="12"/>
       <c r="Q6" s="7"/>
       <c r="R6" s="8"/>
       <c r="S6" s="8"/>
@@ -4922,11 +6933,11 @@
         <v>6</v>
       </c>
       <c r="B8" t="e">
-        <f>AVERAGE(B29,B45,B61,B77,B93)</f>
+        <f>AVERAGE(B29,B54,B70,B86,B102)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="C8" t="e">
-        <f t="shared" ref="C8:AA8" si="0">AVERAGE(C29,C45,C61,C77,C93)</f>
+        <f t="shared" ref="C8:AA8" si="0">AVERAGE(C29,C54,C70,C86,C102)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D8" t="e">
@@ -4934,11 +6945,11 @@
         <v>#DIV/0!</v>
       </c>
       <c r="F8" t="e">
-        <f>AVERAGE(F29,F45,F61,F77,F93)</f>
+        <f>AVERAGE(F29,F54,F70,F86,F102)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="G8" t="e">
-        <f t="shared" ref="G8:H8" si="1">AVERAGE(G29,G45,G61,G77,G93)</f>
+        <f t="shared" ref="G8:H8" si="1">AVERAGE(G29,G54,G70,G86,G102)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="H8" t="e">
@@ -4946,11 +6957,11 @@
         <v>#DIV/0!</v>
       </c>
       <c r="J8" t="e">
-        <f>AVERAGE(J29,J45,J61,J77,J93)</f>
+        <f>AVERAGE(J29,J54,J70,J86,J102)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="K8" t="e">
-        <f t="shared" ref="K8:L8" si="2">AVERAGE(K29,K45,K61,K77,K93)</f>
+        <f t="shared" ref="K8:L8" si="2">AVERAGE(K29,K54,K70,K86,K102)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="L8" t="e">
@@ -4958,11 +6969,11 @@
         <v>#DIV/0!</v>
       </c>
       <c r="N8" t="e">
-        <f>AVERAGE(N29,N45,N61,N77,N93)</f>
+        <f>AVERAGE(N29,N54,N70,N86,N102)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="O8" t="e">
-        <f t="shared" ref="O8:P8" si="3">AVERAGE(O29,O45,O61,O77,O93)</f>
+        <f t="shared" ref="O8:P8" si="3">AVERAGE(O29,O54,O70,O86,O102)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="P8" t="e">
@@ -4975,11 +6986,11 @@
         <v>7</v>
       </c>
       <c r="B9" t="e">
-        <f>AVERAGE(B30,B46,B62,B78,B94)</f>
+        <f>AVERAGE(B30,B55,B71,B87,B103)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="C9" t="e">
-        <f t="shared" ref="C9:AA9" si="4">AVERAGE(C30,C46,C62,C78,C94)</f>
+        <f t="shared" ref="C9:AA9" si="4">AVERAGE(C30,C55,C71,C87,C103)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D9" t="e">
@@ -4987,11 +6998,11 @@
         <v>#DIV/0!</v>
       </c>
       <c r="F9" t="e">
-        <f>AVERAGE(F30,F46,F62,F78,F94)</f>
+        <f>AVERAGE(F30,F55,F71,F87,F103)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="G9" t="e">
-        <f t="shared" ref="G9:H9" si="5">AVERAGE(G30,G46,G62,G78,G94)</f>
+        <f t="shared" ref="G9:H9" si="5">AVERAGE(G30,G55,G71,G87,G103)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="H9" t="e">
@@ -4999,11 +7010,11 @@
         <v>#DIV/0!</v>
       </c>
       <c r="J9" t="e">
-        <f>AVERAGE(J30,J46,J62,J78,J94)</f>
+        <f>AVERAGE(J30,J55,J71,J87,J103)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="K9" t="e">
-        <f t="shared" ref="K9:L9" si="6">AVERAGE(K30,K46,K62,K78,K94)</f>
+        <f t="shared" ref="K9:L9" si="6">AVERAGE(K30,K55,K71,K87,K103)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="L9" t="e">
@@ -5011,11 +7022,11 @@
         <v>#DIV/0!</v>
       </c>
       <c r="N9" t="e">
-        <f>AVERAGE(N30,N46,N62,N78,N94)</f>
+        <f>AVERAGE(N30,N55,N71,N87,N103)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="O9" t="e">
-        <f t="shared" ref="O9:P9" si="7">AVERAGE(O30,O46,O62,O78,O94)</f>
+        <f t="shared" ref="O9:P9" si="7">AVERAGE(O30,O55,O71,O87,O103)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="P9" t="e">
@@ -5035,87 +7046,87 @@
       <c r="O11" s="7"/>
     </row>
     <row r="12" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="12"/>
-      <c r="B12" s="12"/>
+      <c r="A12" s="13"/>
+      <c r="B12" s="13"/>
       <c r="C12" s="9"/>
       <c r="D12" s="6"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
       <c r="G12" s="9"/>
       <c r="H12" s="6"/>
-      <c r="I12" s="12"/>
-      <c r="J12" s="12"/>
+      <c r="I12" s="13"/>
+      <c r="J12" s="13"/>
       <c r="K12" s="9"/>
       <c r="L12" s="6"/>
       <c r="M12" s="6"/>
-      <c r="N12" s="12"/>
+      <c r="N12" s="13"/>
       <c r="O12" s="9"/>
       <c r="P12" s="6"/>
       <c r="Q12" s="6"/>
-      <c r="R12" s="12"/>
-      <c r="S12" s="12"/>
+      <c r="R12" s="13"/>
+      <c r="S12" s="13"/>
       <c r="T12" s="9"/>
       <c r="U12" s="6"/>
-      <c r="V12" s="12"/>
-      <c r="W12" s="12"/>
+      <c r="V12" s="13"/>
+      <c r="W12" s="13"/>
       <c r="X12" s="9"/>
       <c r="Y12" s="6"/>
       <c r="Z12" s="6"/>
       <c r="AA12" s="6"/>
     </row>
     <row r="13" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A13" s="12"/>
-      <c r="B13" s="12"/>
+      <c r="A13" s="13"/>
+      <c r="B13" s="13"/>
       <c r="C13" s="9"/>
       <c r="D13" s="6"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
       <c r="G13" s="9"/>
       <c r="H13" s="6"/>
-      <c r="I13" s="12"/>
-      <c r="J13" s="12"/>
+      <c r="I13" s="13"/>
+      <c r="J13" s="13"/>
       <c r="K13" s="9"/>
       <c r="L13" s="6"/>
       <c r="M13" s="6"/>
-      <c r="N13" s="12"/>
+      <c r="N13" s="13"/>
       <c r="O13" s="9"/>
       <c r="P13" s="6"/>
       <c r="Q13" s="6"/>
-      <c r="R13" s="12"/>
-      <c r="S13" s="12"/>
+      <c r="R13" s="13"/>
+      <c r="S13" s="13"/>
       <c r="T13" s="9"/>
       <c r="U13" s="6"/>
-      <c r="V13" s="12"/>
-      <c r="W13" s="12"/>
+      <c r="V13" s="13"/>
+      <c r="W13" s="13"/>
       <c r="X13" s="9"/>
       <c r="Y13" s="6"/>
       <c r="Z13" s="6"/>
       <c r="AA13" s="6"/>
     </row>
     <row r="14" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A14" s="12"/>
-      <c r="B14" s="12"/>
+      <c r="A14" s="13"/>
+      <c r="B14" s="13"/>
       <c r="C14" s="9"/>
       <c r="D14" s="6"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
       <c r="G14" s="9"/>
       <c r="H14" s="6"/>
-      <c r="I14" s="12"/>
-      <c r="J14" s="12"/>
+      <c r="I14" s="13"/>
+      <c r="J14" s="13"/>
       <c r="K14" s="9"/>
       <c r="L14" s="6"/>
       <c r="M14" s="6"/>
-      <c r="N14" s="12"/>
+      <c r="N14" s="13"/>
       <c r="O14" s="9"/>
       <c r="P14" s="6"/>
       <c r="Q14" s="6"/>
-      <c r="R14" s="12"/>
-      <c r="S14" s="12"/>
+      <c r="R14" s="13"/>
+      <c r="S14" s="13"/>
       <c r="T14" s="9"/>
       <c r="U14" s="6"/>
-      <c r="V14" s="12"/>
-      <c r="W14" s="12"/>
+      <c r="V14" s="13"/>
+      <c r="W14" s="13"/>
       <c r="X14" s="9"/>
       <c r="Y14" s="6"/>
       <c r="Z14" s="6"/>
@@ -5141,29 +7152,29 @@
       <c r="A17" t="s">
         <v>0</v>
       </c>
-      <c r="B17" s="11" t="s">
+      <c r="B17" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="12"/>
       <c r="E17" s="7"/>
-      <c r="F17" s="11" t="s">
+      <c r="F17" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="G17" s="11"/>
-      <c r="H17" s="11"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="12"/>
       <c r="I17" s="8"/>
-      <c r="J17" s="11" t="s">
+      <c r="J17" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="K17" s="11"/>
-      <c r="L17" s="11"/>
+      <c r="K17" s="12"/>
+      <c r="L17" s="12"/>
       <c r="M17" s="8"/>
-      <c r="N17" s="11" t="s">
+      <c r="N17" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="O17" s="11"/>
-      <c r="P17" s="11"/>
+      <c r="O17" s="12"/>
+      <c r="P17" s="12"/>
       <c r="R17" s="8"/>
       <c r="S17" s="8"/>
       <c r="T17" s="8"/>
@@ -5640,1048 +7651,1132 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="31" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="B31" s="8"/>
-      <c r="C31" s="8"/>
-      <c r="D31" s="1"/>
-      <c r="E31" s="7"/>
-      <c r="F31" s="8"/>
-      <c r="G31" s="8"/>
-      <c r="H31" s="1"/>
-      <c r="I31" s="8"/>
-      <c r="J31" s="8"/>
-      <c r="K31" s="8"/>
-      <c r="L31" s="1"/>
-      <c r="M31" s="7"/>
-      <c r="N31" s="8"/>
-      <c r="O31" s="8"/>
-      <c r="P31" s="1"/>
-      <c r="Q31" s="7"/>
-      <c r="R31" s="7"/>
-      <c r="S31" s="7"/>
-      <c r="T31" s="7"/>
-      <c r="U31" s="7"/>
-      <c r="V31" s="7"/>
-      <c r="W31" s="7"/>
-      <c r="X31" s="7"/>
-      <c r="Y31" s="7"/>
-      <c r="Z31" s="7"/>
-    </row>
     <row r="32" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+      <c r="B32" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C32" s="10"/>
+      <c r="D32" s="11">
+        <f>(F29-B29)/B29</f>
+        <v>3.7352077213596311</v>
+      </c>
+      <c r="F32" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="G32" s="10"/>
+      <c r="H32" s="11">
+        <f>(J29-F29)/F29</f>
+        <v>7.8870967741935498</v>
+      </c>
+    </row>
+    <row r="33" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="10"/>
+      <c r="C33" s="10"/>
+      <c r="D33" s="11"/>
+      <c r="F33" s="10"/>
+      <c r="G33" s="10"/>
+      <c r="H33" s="11"/>
+    </row>
+    <row r="34" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="B34" s="10"/>
+      <c r="C34" s="10"/>
+      <c r="D34" s="11"/>
+      <c r="F34" s="10"/>
+      <c r="G34" s="10"/>
+      <c r="H34" s="11"/>
+    </row>
+    <row r="35" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="B35" s="8"/>
+      <c r="C35" s="8"/>
+      <c r="D35" s="9"/>
+      <c r="F35" s="8"/>
+      <c r="G35" s="8"/>
+      <c r="H35" s="9"/>
+    </row>
+    <row r="36" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="B36" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C36" s="10"/>
+      <c r="D36" s="11">
+        <f>(D29-H29)/H29</f>
+        <v>0.38727449875207098</v>
+      </c>
+      <c r="F36" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="G36" s="10"/>
+      <c r="H36" s="11">
+        <f>(H29-L29)/L29</f>
+        <v>0.40410272186946139</v>
+      </c>
+    </row>
+    <row r="37" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="B37" s="10"/>
+      <c r="C37" s="10"/>
+      <c r="D37" s="11"/>
+      <c r="F37" s="10"/>
+      <c r="G37" s="10"/>
+      <c r="H37" s="11"/>
+    </row>
+    <row r="38" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="B38" s="10"/>
+      <c r="C38" s="10"/>
+      <c r="D38" s="11"/>
+      <c r="F38" s="10"/>
+      <c r="G38" s="10"/>
+      <c r="H38" s="11"/>
+    </row>
+    <row r="40" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="B40" s="8"/>
+      <c r="C40" s="8"/>
+      <c r="D40" s="1"/>
+      <c r="E40" s="7"/>
+      <c r="F40" s="8"/>
+      <c r="G40" s="8"/>
+      <c r="H40" s="1"/>
+      <c r="I40" s="8"/>
+      <c r="J40" s="8"/>
+      <c r="K40" s="8"/>
+      <c r="L40" s="1"/>
+      <c r="M40" s="7"/>
+      <c r="N40" s="8"/>
+      <c r="O40" s="8"/>
+      <c r="P40" s="1"/>
+      <c r="Q40" s="7"/>
+      <c r="R40" s="7"/>
+      <c r="S40" s="7"/>
+      <c r="T40" s="7"/>
+      <c r="U40" s="7"/>
+      <c r="V40" s="7"/>
+      <c r="W40" s="7"/>
+      <c r="X40" s="7"/>
+      <c r="Y40" s="7"/>
+      <c r="Z40" s="7"/>
+    </row>
+    <row r="41" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>4</v>
       </c>
-      <c r="M32" s="7"/>
-      <c r="Q32" s="7"/>
-      <c r="R32" s="7"/>
-      <c r="S32" s="7"/>
-      <c r="T32" s="7"/>
-      <c r="U32" s="7"/>
-      <c r="V32" s="7"/>
-      <c r="W32" s="7"/>
-      <c r="X32" s="7"/>
-      <c r="Y32" s="7"/>
-      <c r="Z32" s="7"/>
-    </row>
-    <row r="33" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+      <c r="M41" s="7"/>
+      <c r="Q41" s="7"/>
+      <c r="R41" s="7"/>
+      <c r="S41" s="7"/>
+      <c r="T41" s="7"/>
+      <c r="U41" s="7"/>
+      <c r="V41" s="7"/>
+      <c r="W41" s="7"/>
+      <c r="X41" s="7"/>
+      <c r="Y41" s="7"/>
+      <c r="Z41" s="7"/>
+    </row>
+    <row r="42" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>0</v>
       </c>
-      <c r="B33" s="11" t="s">
+      <c r="B42" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="C33" s="11"/>
-      <c r="D33" s="11"/>
-      <c r="E33" s="7"/>
-      <c r="F33" s="11" t="s">
+      <c r="C42" s="12"/>
+      <c r="D42" s="12"/>
+      <c r="E42" s="7"/>
+      <c r="F42" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="G33" s="11"/>
-      <c r="H33" s="11"/>
-      <c r="I33" s="8"/>
-      <c r="J33" s="11" t="s">
+      <c r="G42" s="12"/>
+      <c r="H42" s="12"/>
+      <c r="I42" s="8"/>
+      <c r="J42" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="K33" s="11"/>
-      <c r="L33" s="11"/>
-      <c r="M33" s="8"/>
-      <c r="N33" s="11" t="s">
+      <c r="K42" s="12"/>
+      <c r="L42" s="12"/>
+      <c r="M42" s="8"/>
+      <c r="N42" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="O33" s="11"/>
-      <c r="P33" s="11"/>
-      <c r="R33" s="8"/>
-      <c r="S33" s="8"/>
-      <c r="T33" s="8"/>
-      <c r="U33" s="8"/>
-      <c r="V33" s="8"/>
-      <c r="W33" s="8"/>
-      <c r="X33" s="8"/>
-      <c r="Y33" s="8"/>
-      <c r="Z33" s="8"/>
-      <c r="AA33" s="8"/>
-    </row>
-    <row r="34" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="B34" t="s">
+      <c r="O42" s="12"/>
+      <c r="P42" s="12"/>
+      <c r="R42" s="8"/>
+      <c r="S42" s="8"/>
+      <c r="T42" s="8"/>
+      <c r="U42" s="8"/>
+      <c r="V42" s="8"/>
+      <c r="W42" s="8"/>
+      <c r="X42" s="8"/>
+      <c r="Y42" s="8"/>
+      <c r="Z42" s="8"/>
+      <c r="AA42" s="8"/>
+    </row>
+    <row r="43" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
         <v>12</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C43" t="s">
         <v>13</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D43" t="s">
         <v>14</v>
       </c>
-      <c r="F34" t="s">
+      <c r="F43" t="s">
         <v>12</v>
       </c>
-      <c r="G34" t="s">
+      <c r="G43" t="s">
         <v>13</v>
       </c>
-      <c r="H34" t="s">
+      <c r="H43" t="s">
         <v>14</v>
       </c>
-      <c r="J34" t="s">
+      <c r="J43" t="s">
         <v>12</v>
       </c>
-      <c r="K34" t="s">
+      <c r="K43" t="s">
         <v>13</v>
       </c>
-      <c r="L34" t="s">
+      <c r="L43" t="s">
         <v>14</v>
       </c>
-      <c r="N34" t="s">
+      <c r="N43" t="s">
         <v>12</v>
       </c>
-      <c r="O34" t="s">
+      <c r="O43" t="s">
         <v>13</v>
       </c>
-      <c r="P34" t="s">
+      <c r="P43" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="35" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A35">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="37" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A37">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="38" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A38">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="39" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A39">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="40" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A40">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="41" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A41">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="42" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A42">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="43" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A43">
-        <v>9</v>
       </c>
     </row>
     <row r="44" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="45" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>1</v>
-      </c>
-      <c r="B45" t="e">
-        <f t="shared" ref="B45" si="13">AVERAGE(B35:B44)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C45" t="e">
-        <f t="shared" ref="C45" si="14">AVERAGE(C35:C44)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D45" t="e">
-        <f t="shared" ref="D45" si="15">AVERAGE(D35:D44)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F45" t="e">
-        <f t="shared" ref="F45:H45" si="16">AVERAGE(F35:F44)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G45" t="e">
-        <f t="shared" si="16"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H45" t="e">
-        <f t="shared" si="16"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J45" t="e">
-        <f t="shared" ref="J45:L45" si="17">AVERAGE(J35:J44)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K45" t="e">
-        <f t="shared" si="17"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L45" t="e">
-        <f t="shared" si="17"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N45" t="e">
-        <f t="shared" ref="N45:P45" si="18">AVERAGE(N35:N44)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O45" t="e">
-        <f t="shared" si="18"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P45" t="e">
-        <f t="shared" si="18"/>
-        <v>#DIV/0!</v>
+      <c r="A45">
+        <v>2</v>
       </c>
     </row>
     <row r="46" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+      <c r="A46">
         <v>3</v>
       </c>
-      <c r="B46" t="e">
-        <f>STDEV(B35:B44)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C46" t="e">
-        <f>STDEV(C35:C44)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D46" t="e">
-        <f t="shared" ref="D46" si="19">STDEV(D35:D44)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F46" t="e">
-        <f>STDEV(F35:F44)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G46" t="e">
-        <f>STDEV(G35:G44)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H46" t="e">
-        <f t="shared" ref="H46" si="20">STDEV(H35:H44)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J46" t="e">
-        <f>STDEV(J35:J44)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K46" t="e">
-        <f>STDEV(K35:K44)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L46" t="e">
-        <f t="shared" ref="L46" si="21">STDEV(L35:L44)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N46" t="e">
-        <f>STDEV(N35:N44)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O46" t="e">
-        <f>STDEV(O35:O44)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P46" t="e">
-        <f t="shared" ref="P46" si="22">STDEV(P35:P44)</f>
-        <v>#DIV/0!</v>
+    </row>
+    <row r="47" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>4</v>
       </c>
     </row>
     <row r="48" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
+      <c r="A48">
         <v>5</v>
       </c>
-      <c r="M48" s="7"/>
-      <c r="Q48" s="7"/>
-      <c r="R48" s="7"/>
-      <c r="S48" s="7"/>
-      <c r="T48" s="7"/>
-      <c r="U48" s="7"/>
-      <c r="V48" s="7"/>
-      <c r="W48" s="7"/>
-      <c r="X48" s="7"/>
-      <c r="Y48" s="7"/>
-      <c r="Z48" s="7"/>
     </row>
     <row r="49" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>0</v>
-      </c>
-      <c r="B49" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="C49" s="11"/>
-      <c r="D49" s="11"/>
-      <c r="E49" s="7"/>
-      <c r="F49" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="G49" s="11"/>
-      <c r="H49" s="11"/>
-      <c r="I49" s="8"/>
-      <c r="J49" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="K49" s="11"/>
-      <c r="L49" s="11"/>
-      <c r="M49" s="8"/>
-      <c r="N49" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="O49" s="11"/>
-      <c r="P49" s="11"/>
-      <c r="R49" s="8"/>
-      <c r="S49" s="8"/>
-      <c r="T49" s="8"/>
-      <c r="U49" s="8"/>
-      <c r="V49" s="8"/>
-      <c r="W49" s="8"/>
-      <c r="X49" s="8"/>
-      <c r="Y49" s="8"/>
-      <c r="Z49" s="8"/>
-      <c r="AA49" s="8"/>
+      <c r="A49">
+        <v>6</v>
+      </c>
     </row>
     <row r="50" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="B50" t="s">
-        <v>12</v>
-      </c>
-      <c r="C50" t="s">
-        <v>13</v>
-      </c>
-      <c r="D50" t="s">
-        <v>14</v>
-      </c>
-      <c r="F50" t="s">
-        <v>12</v>
-      </c>
-      <c r="G50" t="s">
-        <v>13</v>
-      </c>
-      <c r="H50" t="s">
-        <v>14</v>
-      </c>
-      <c r="J50" t="s">
-        <v>12</v>
-      </c>
-      <c r="K50" t="s">
-        <v>13</v>
-      </c>
-      <c r="L50" t="s">
-        <v>14</v>
-      </c>
-      <c r="N50" t="s">
-        <v>12</v>
-      </c>
-      <c r="O50" t="s">
-        <v>13</v>
-      </c>
-      <c r="P50" t="s">
-        <v>14</v>
+      <c r="A50">
+        <v>7</v>
       </c>
     </row>
     <row r="51" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="52" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>2</v>
+        <v>9</v>
       </c>
     </row>
     <row r="53" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A53">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="54" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>1</v>
+      </c>
+      <c r="B54" t="e">
+        <f t="shared" ref="B54" si="13">AVERAGE(B44:B53)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C54" t="e">
+        <f t="shared" ref="C54" si="14">AVERAGE(C44:C53)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D54" t="e">
+        <f t="shared" ref="D54" si="15">AVERAGE(D44:D53)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F54" t="e">
+        <f t="shared" ref="F54:H54" si="16">AVERAGE(F44:F53)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G54" t="e">
+        <f t="shared" si="16"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H54" t="e">
+        <f t="shared" si="16"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J54" t="e">
+        <f t="shared" ref="J54:L54" si="17">AVERAGE(J44:J53)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K54" t="e">
+        <f t="shared" si="17"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L54" t="e">
+        <f t="shared" si="17"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N54" t="e">
+        <f t="shared" ref="N54:P54" si="18">AVERAGE(N44:N53)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O54" t="e">
+        <f t="shared" si="18"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P54" t="e">
+        <f t="shared" si="18"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="55" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="54" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A54">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="55" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A55">
+      <c r="B55" t="e">
+        <f>STDEV(B44:B53)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C55" t="e">
+        <f>STDEV(C44:C53)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D55" t="e">
+        <f t="shared" ref="D55" si="19">STDEV(D44:D53)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F55" t="e">
+        <f>STDEV(F44:F53)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G55" t="e">
+        <f>STDEV(G44:G53)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H55" t="e">
+        <f t="shared" ref="H55" si="20">STDEV(H44:H53)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J55" t="e">
+        <f>STDEV(J44:J53)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K55" t="e">
+        <f>STDEV(K44:K53)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L55" t="e">
+        <f t="shared" ref="L55" si="21">STDEV(L44:L53)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N55" t="e">
+        <f>STDEV(N44:N53)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O55" t="e">
+        <f>STDEV(O44:O53)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P55" t="e">
+        <f t="shared" ref="P55" si="22">STDEV(P44:P53)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="57" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="56" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A56">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="57" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A57">
-        <v>7</v>
-      </c>
+      <c r="M57" s="7"/>
+      <c r="Q57" s="7"/>
+      <c r="R57" s="7"/>
+      <c r="S57" s="7"/>
+      <c r="T57" s="7"/>
+      <c r="U57" s="7"/>
+      <c r="V57" s="7"/>
+      <c r="W57" s="7"/>
+      <c r="X57" s="7"/>
+      <c r="Y57" s="7"/>
+      <c r="Z57" s="7"/>
     </row>
     <row r="58" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A58">
-        <v>8</v>
-      </c>
+      <c r="A58" t="s">
+        <v>0</v>
+      </c>
+      <c r="B58" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C58" s="12"/>
+      <c r="D58" s="12"/>
+      <c r="E58" s="7"/>
+      <c r="F58" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="G58" s="12"/>
+      <c r="H58" s="12"/>
+      <c r="I58" s="8"/>
+      <c r="J58" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="K58" s="12"/>
+      <c r="L58" s="12"/>
+      <c r="M58" s="8"/>
+      <c r="N58" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="O58" s="12"/>
+      <c r="P58" s="12"/>
+      <c r="R58" s="8"/>
+      <c r="S58" s="8"/>
+      <c r="T58" s="8"/>
+      <c r="U58" s="8"/>
+      <c r="V58" s="8"/>
+      <c r="W58" s="8"/>
+      <c r="X58" s="8"/>
+      <c r="Y58" s="8"/>
+      <c r="Z58" s="8"/>
+      <c r="AA58" s="8"/>
     </row>
     <row r="59" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A59">
-        <v>9</v>
+      <c r="B59" t="s">
+        <v>12</v>
+      </c>
+      <c r="C59" t="s">
+        <v>13</v>
+      </c>
+      <c r="D59" t="s">
+        <v>14</v>
+      </c>
+      <c r="F59" t="s">
+        <v>12</v>
+      </c>
+      <c r="G59" t="s">
+        <v>13</v>
+      </c>
+      <c r="H59" t="s">
+        <v>14</v>
+      </c>
+      <c r="J59" t="s">
+        <v>12</v>
+      </c>
+      <c r="K59" t="s">
+        <v>13</v>
+      </c>
+      <c r="L59" t="s">
+        <v>14</v>
+      </c>
+      <c r="N59" t="s">
+        <v>12</v>
+      </c>
+      <c r="O59" t="s">
+        <v>13</v>
+      </c>
+      <c r="P59" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="60" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A60">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="61" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>1</v>
-      </c>
-      <c r="B61" t="e">
-        <f t="shared" ref="B61" si="23">AVERAGE(B51:B60)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C61" t="e">
-        <f t="shared" ref="C61" si="24">AVERAGE(C51:C60)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D61" t="e">
-        <f t="shared" ref="D61" si="25">AVERAGE(D51:D60)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F61" t="e">
-        <f t="shared" ref="F61:H61" si="26">AVERAGE(F51:F60)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G61" t="e">
-        <f t="shared" si="26"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H61" t="e">
-        <f t="shared" si="26"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J61" t="e">
-        <f t="shared" ref="J61:L61" si="27">AVERAGE(J51:J60)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K61" t="e">
-        <f t="shared" si="27"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L61" t="e">
-        <f t="shared" si="27"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N61" t="e">
-        <f t="shared" ref="N61:P61" si="28">AVERAGE(N51:N60)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O61" t="e">
-        <f t="shared" si="28"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P61" t="e">
-        <f t="shared" si="28"/>
-        <v>#DIV/0!</v>
+      <c r="A61">
+        <v>2</v>
       </c>
     </row>
     <row r="62" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
+      <c r="A62">
         <v>3</v>
       </c>
-      <c r="B62" t="e">
-        <f>STDEV(B51:B60)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C62" t="e">
-        <f>STDEV(C51:C60)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D62" t="e">
-        <f t="shared" ref="D62" si="29">STDEV(D51:D60)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F62" t="e">
-        <f>STDEV(F51:F60)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G62" t="e">
-        <f>STDEV(G51:G60)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H62" t="e">
-        <f t="shared" ref="H62" si="30">STDEV(H51:H60)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J62" t="e">
-        <f>STDEV(J51:J60)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K62" t="e">
-        <f>STDEV(K51:K60)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L62" t="e">
-        <f t="shared" ref="L62" si="31">STDEV(L51:L60)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N62" t="e">
-        <f>STDEV(N51:N60)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O62" t="e">
-        <f>STDEV(O51:O60)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P62" t="e">
-        <f t="shared" ref="P62" si="32">STDEV(P51:P60)</f>
-        <v>#DIV/0!</v>
+    </row>
+    <row r="63" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>4</v>
       </c>
     </row>
     <row r="64" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>9</v>
-      </c>
-      <c r="M64" s="7"/>
-      <c r="Q64" s="7"/>
-      <c r="R64" s="7"/>
-      <c r="S64" s="7"/>
-      <c r="T64" s="7"/>
-      <c r="U64" s="7"/>
-      <c r="V64" s="7"/>
-      <c r="W64" s="7"/>
-      <c r="X64" s="7"/>
-      <c r="Y64" s="7"/>
-      <c r="Z64" s="7"/>
+      <c r="A64">
+        <v>5</v>
+      </c>
     </row>
     <row r="65" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>0</v>
-      </c>
-      <c r="B65" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="C65" s="11"/>
-      <c r="D65" s="11"/>
-      <c r="E65" s="7"/>
-      <c r="F65" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="G65" s="11"/>
-      <c r="H65" s="11"/>
-      <c r="I65" s="8"/>
-      <c r="J65" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="K65" s="11"/>
-      <c r="L65" s="11"/>
-      <c r="M65" s="8"/>
-      <c r="N65" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="O65" s="11"/>
-      <c r="P65" s="11"/>
-      <c r="R65" s="8"/>
-      <c r="S65" s="8"/>
-      <c r="T65" s="8"/>
-      <c r="U65" s="8"/>
-      <c r="V65" s="8"/>
-      <c r="W65" s="8"/>
-      <c r="X65" s="8"/>
-      <c r="Y65" s="8"/>
-      <c r="Z65" s="8"/>
-      <c r="AA65" s="8"/>
+      <c r="A65">
+        <v>6</v>
+      </c>
     </row>
     <row r="66" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="B66" t="s">
-        <v>12</v>
-      </c>
-      <c r="C66" t="s">
-        <v>13</v>
-      </c>
-      <c r="D66" t="s">
-        <v>14</v>
-      </c>
-      <c r="F66" t="s">
-        <v>12</v>
-      </c>
-      <c r="G66" t="s">
-        <v>13</v>
-      </c>
-      <c r="H66" t="s">
-        <v>14</v>
-      </c>
-      <c r="J66" t="s">
-        <v>12</v>
-      </c>
-      <c r="K66" t="s">
-        <v>13</v>
-      </c>
-      <c r="L66" t="s">
-        <v>14</v>
-      </c>
-      <c r="N66" t="s">
-        <v>12</v>
-      </c>
-      <c r="O66" t="s">
-        <v>13</v>
-      </c>
-      <c r="P66" t="s">
-        <v>14</v>
+      <c r="A66">
+        <v>7</v>
       </c>
     </row>
     <row r="67" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A67">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="68" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A68">
-        <v>2</v>
+        <v>9</v>
       </c>
     </row>
     <row r="69" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A69">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="70" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>1</v>
+      </c>
+      <c r="B70" t="e">
+        <f t="shared" ref="B70" si="23">AVERAGE(B60:B69)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C70" t="e">
+        <f t="shared" ref="C70" si="24">AVERAGE(C60:C69)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D70" t="e">
+        <f t="shared" ref="D70" si="25">AVERAGE(D60:D69)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F70" t="e">
+        <f t="shared" ref="F70:H70" si="26">AVERAGE(F60:F69)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G70" t="e">
+        <f t="shared" si="26"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H70" t="e">
+        <f t="shared" si="26"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J70" t="e">
+        <f t="shared" ref="J70:L70" si="27">AVERAGE(J60:J69)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K70" t="e">
+        <f t="shared" si="27"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L70" t="e">
+        <f t="shared" si="27"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N70" t="e">
+        <f t="shared" ref="N70:P70" si="28">AVERAGE(N60:N69)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O70" t="e">
+        <f t="shared" si="28"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P70" t="e">
+        <f t="shared" si="28"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="71" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="70" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A70">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="71" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A71">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="72" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A72">
-        <v>6</v>
+      <c r="B71" t="e">
+        <f>STDEV(B60:B69)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C71" t="e">
+        <f>STDEV(C60:C69)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D71" t="e">
+        <f t="shared" ref="D71" si="29">STDEV(D60:D69)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F71" t="e">
+        <f>STDEV(F60:F69)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G71" t="e">
+        <f>STDEV(G60:G69)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H71" t="e">
+        <f t="shared" ref="H71" si="30">STDEV(H60:H69)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J71" t="e">
+        <f>STDEV(J60:J69)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K71" t="e">
+        <f>STDEV(K60:K69)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L71" t="e">
+        <f t="shared" ref="L71" si="31">STDEV(L60:L69)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N71" t="e">
+        <f>STDEV(N60:N69)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O71" t="e">
+        <f>STDEV(O60:O69)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P71" t="e">
+        <f t="shared" ref="P71" si="32">STDEV(P60:P69)</f>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="73" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A73">
-        <v>7</v>
-      </c>
+      <c r="A73" t="s">
+        <v>9</v>
+      </c>
+      <c r="M73" s="7"/>
+      <c r="Q73" s="7"/>
+      <c r="R73" s="7"/>
+      <c r="S73" s="7"/>
+      <c r="T73" s="7"/>
+      <c r="U73" s="7"/>
+      <c r="V73" s="7"/>
+      <c r="W73" s="7"/>
+      <c r="X73" s="7"/>
+      <c r="Y73" s="7"/>
+      <c r="Z73" s="7"/>
     </row>
     <row r="74" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A74">
-        <v>8</v>
-      </c>
+      <c r="A74" t="s">
+        <v>0</v>
+      </c>
+      <c r="B74" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C74" s="12"/>
+      <c r="D74" s="12"/>
+      <c r="E74" s="7"/>
+      <c r="F74" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="G74" s="12"/>
+      <c r="H74" s="12"/>
+      <c r="I74" s="8"/>
+      <c r="J74" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="K74" s="12"/>
+      <c r="L74" s="12"/>
+      <c r="M74" s="8"/>
+      <c r="N74" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="O74" s="12"/>
+      <c r="P74" s="12"/>
+      <c r="R74" s="8"/>
+      <c r="S74" s="8"/>
+      <c r="T74" s="8"/>
+      <c r="U74" s="8"/>
+      <c r="V74" s="8"/>
+      <c r="W74" s="8"/>
+      <c r="X74" s="8"/>
+      <c r="Y74" s="8"/>
+      <c r="Z74" s="8"/>
+      <c r="AA74" s="8"/>
     </row>
     <row r="75" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A75">
-        <v>9</v>
+      <c r="B75" t="s">
+        <v>12</v>
+      </c>
+      <c r="C75" t="s">
+        <v>13</v>
+      </c>
+      <c r="D75" t="s">
+        <v>14</v>
+      </c>
+      <c r="F75" t="s">
+        <v>12</v>
+      </c>
+      <c r="G75" t="s">
+        <v>13</v>
+      </c>
+      <c r="H75" t="s">
+        <v>14</v>
+      </c>
+      <c r="J75" t="s">
+        <v>12</v>
+      </c>
+      <c r="K75" t="s">
+        <v>13</v>
+      </c>
+      <c r="L75" t="s">
+        <v>14</v>
+      </c>
+      <c r="N75" t="s">
+        <v>12</v>
+      </c>
+      <c r="O75" t="s">
+        <v>13</v>
+      </c>
+      <c r="P75" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="76" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A76">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="77" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
-        <v>1</v>
-      </c>
-      <c r="B77" t="e">
-        <f t="shared" ref="B77" si="33">AVERAGE(B67:B76)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C77" t="e">
-        <f t="shared" ref="C77" si="34">AVERAGE(C67:C76)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D77" t="e">
-        <f t="shared" ref="D77" si="35">AVERAGE(D67:D76)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F77" t="e">
-        <f t="shared" ref="F77:H77" si="36">AVERAGE(F67:F76)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G77" t="e">
-        <f t="shared" si="36"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H77" t="e">
-        <f t="shared" si="36"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J77" t="e">
-        <f t="shared" ref="J77:L77" si="37">AVERAGE(J67:J76)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K77" t="e">
-        <f t="shared" si="37"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L77" t="e">
-        <f t="shared" si="37"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N77" t="e">
-        <f t="shared" ref="N77:P77" si="38">AVERAGE(N67:N76)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O77" t="e">
-        <f t="shared" si="38"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P77" t="e">
-        <f t="shared" si="38"/>
-        <v>#DIV/0!</v>
+      <c r="A77">
+        <v>2</v>
       </c>
     </row>
     <row r="78" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
+      <c r="A78">
         <v>3</v>
       </c>
-      <c r="B78" t="e">
-        <f>STDEV(B67:B76)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C78" t="e">
-        <f>STDEV(C67:C76)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D78" t="e">
-        <f t="shared" ref="D78" si="39">STDEV(D67:D76)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F78" t="e">
-        <f>STDEV(F67:F76)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G78" t="e">
-        <f>STDEV(G67:G76)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H78" t="e">
-        <f t="shared" ref="H78" si="40">STDEV(H67:H76)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J78" t="e">
-        <f>STDEV(J67:J76)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K78" t="e">
-        <f>STDEV(K67:K76)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L78" t="e">
-        <f t="shared" ref="L78" si="41">STDEV(L67:L76)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N78" t="e">
-        <f>STDEV(N67:N76)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O78" t="e">
-        <f>STDEV(O67:O76)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P78" t="e">
-        <f t="shared" ref="P78" si="42">STDEV(P67:P76)</f>
-        <v>#DIV/0!</v>
+    </row>
+    <row r="79" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>4</v>
       </c>
     </row>
     <row r="80" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
-        <v>8</v>
-      </c>
-      <c r="M80" s="7"/>
-      <c r="Q80" s="7"/>
-      <c r="R80" s="7"/>
-      <c r="S80" s="7"/>
-      <c r="T80" s="7"/>
-      <c r="U80" s="7"/>
-      <c r="V80" s="7"/>
-      <c r="W80" s="7"/>
-      <c r="X80" s="7"/>
-      <c r="Y80" s="7"/>
-      <c r="Z80" s="7"/>
+      <c r="A80">
+        <v>5</v>
+      </c>
     </row>
     <row r="81" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
-        <v>0</v>
-      </c>
-      <c r="B81" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="C81" s="11"/>
-      <c r="D81" s="11"/>
-      <c r="E81" s="7"/>
-      <c r="F81" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="G81" s="11"/>
-      <c r="H81" s="11"/>
-      <c r="I81" s="8"/>
-      <c r="J81" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="K81" s="11"/>
-      <c r="L81" s="11"/>
-      <c r="M81" s="8"/>
-      <c r="N81" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="O81" s="11"/>
-      <c r="P81" s="11"/>
-      <c r="R81" s="8"/>
-      <c r="S81" s="8"/>
-      <c r="T81" s="8"/>
-      <c r="U81" s="8"/>
-      <c r="V81" s="8"/>
-      <c r="W81" s="8"/>
-      <c r="X81" s="8"/>
-      <c r="Y81" s="8"/>
-      <c r="Z81" s="8"/>
-      <c r="AA81" s="8"/>
+      <c r="A81">
+        <v>6</v>
+      </c>
     </row>
     <row r="82" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="B82" t="s">
-        <v>12</v>
-      </c>
-      <c r="C82" t="s">
-        <v>13</v>
-      </c>
-      <c r="D82" t="s">
-        <v>14</v>
-      </c>
-      <c r="F82" t="s">
-        <v>12</v>
-      </c>
-      <c r="G82" t="s">
-        <v>13</v>
-      </c>
-      <c r="H82" t="s">
-        <v>14</v>
-      </c>
-      <c r="J82" t="s">
-        <v>12</v>
-      </c>
-      <c r="K82" t="s">
-        <v>13</v>
-      </c>
-      <c r="L82" t="s">
-        <v>14</v>
-      </c>
-      <c r="N82" t="s">
-        <v>12</v>
-      </c>
-      <c r="O82" t="s">
-        <v>13</v>
-      </c>
-      <c r="P82" t="s">
-        <v>14</v>
+      <c r="A82">
+        <v>7</v>
       </c>
     </row>
     <row r="83" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A83">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="84" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A84">
-        <v>2</v>
+        <v>9</v>
       </c>
     </row>
     <row r="85" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A85">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="86" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>1</v>
+      </c>
+      <c r="B86" t="e">
+        <f t="shared" ref="B86" si="33">AVERAGE(B76:B85)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C86" t="e">
+        <f t="shared" ref="C86" si="34">AVERAGE(C76:C85)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D86" t="e">
+        <f t="shared" ref="D86" si="35">AVERAGE(D76:D85)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F86" t="e">
+        <f t="shared" ref="F86:H86" si="36">AVERAGE(F76:F85)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G86" t="e">
+        <f t="shared" si="36"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H86" t="e">
+        <f t="shared" si="36"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J86" t="e">
+        <f t="shared" ref="J86:L86" si="37">AVERAGE(J76:J85)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K86" t="e">
+        <f t="shared" si="37"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L86" t="e">
+        <f t="shared" si="37"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N86" t="e">
+        <f t="shared" ref="N86:P86" si="38">AVERAGE(N76:N85)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O86" t="e">
+        <f t="shared" si="38"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P86" t="e">
+        <f t="shared" si="38"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="87" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="86" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A86">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="87" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A87">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="88" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A88">
-        <v>6</v>
+      <c r="B87" t="e">
+        <f>STDEV(B76:B85)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C87" t="e">
+        <f>STDEV(C76:C85)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D87" t="e">
+        <f t="shared" ref="D87" si="39">STDEV(D76:D85)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F87" t="e">
+        <f>STDEV(F76:F85)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G87" t="e">
+        <f>STDEV(G76:G85)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H87" t="e">
+        <f t="shared" ref="H87" si="40">STDEV(H76:H85)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J87" t="e">
+        <f>STDEV(J76:J85)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K87" t="e">
+        <f>STDEV(K76:K85)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L87" t="e">
+        <f t="shared" ref="L87" si="41">STDEV(L76:L85)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N87" t="e">
+        <f>STDEV(N76:N85)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O87" t="e">
+        <f>STDEV(O76:O85)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P87" t="e">
+        <f t="shared" ref="P87" si="42">STDEV(P76:P85)</f>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="89" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A89">
-        <v>7</v>
-      </c>
+      <c r="A89" t="s">
+        <v>8</v>
+      </c>
+      <c r="M89" s="7"/>
+      <c r="Q89" s="7"/>
+      <c r="R89" s="7"/>
+      <c r="S89" s="7"/>
+      <c r="T89" s="7"/>
+      <c r="U89" s="7"/>
+      <c r="V89" s="7"/>
+      <c r="W89" s="7"/>
+      <c r="X89" s="7"/>
+      <c r="Y89" s="7"/>
+      <c r="Z89" s="7"/>
     </row>
     <row r="90" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A90">
-        <v>8</v>
-      </c>
+      <c r="A90" t="s">
+        <v>0</v>
+      </c>
+      <c r="B90" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C90" s="12"/>
+      <c r="D90" s="12"/>
+      <c r="E90" s="7"/>
+      <c r="F90" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="G90" s="12"/>
+      <c r="H90" s="12"/>
+      <c r="I90" s="8"/>
+      <c r="J90" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="K90" s="12"/>
+      <c r="L90" s="12"/>
+      <c r="M90" s="8"/>
+      <c r="N90" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="O90" s="12"/>
+      <c r="P90" s="12"/>
+      <c r="R90" s="8"/>
+      <c r="S90" s="8"/>
+      <c r="T90" s="8"/>
+      <c r="U90" s="8"/>
+      <c r="V90" s="8"/>
+      <c r="W90" s="8"/>
+      <c r="X90" s="8"/>
+      <c r="Y90" s="8"/>
+      <c r="Z90" s="8"/>
+      <c r="AA90" s="8"/>
     </row>
     <row r="91" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A91">
-        <v>9</v>
+      <c r="B91" t="s">
+        <v>12</v>
+      </c>
+      <c r="C91" t="s">
+        <v>13</v>
+      </c>
+      <c r="D91" t="s">
+        <v>14</v>
+      </c>
+      <c r="F91" t="s">
+        <v>12</v>
+      </c>
+      <c r="G91" t="s">
+        <v>13</v>
+      </c>
+      <c r="H91" t="s">
+        <v>14</v>
+      </c>
+      <c r="J91" t="s">
+        <v>12</v>
+      </c>
+      <c r="K91" t="s">
+        <v>13</v>
+      </c>
+      <c r="L91" t="s">
+        <v>14</v>
+      </c>
+      <c r="N91" t="s">
+        <v>12</v>
+      </c>
+      <c r="O91" t="s">
+        <v>13</v>
+      </c>
+      <c r="P91" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="92" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A92">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="94" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="95" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="96" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="97" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="98" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="99" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="100" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="101" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A101">
         <v>10</v>
       </c>
     </row>
-    <row r="93" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
+    <row r="102" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
         <v>1</v>
       </c>
-      <c r="B93" t="e">
-        <f t="shared" ref="B93" si="43">AVERAGE(B83:B92)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C93" t="e">
-        <f t="shared" ref="C93" si="44">AVERAGE(C83:C92)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D93" t="e">
-        <f t="shared" ref="D93" si="45">AVERAGE(D83:D92)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F93" t="e">
-        <f t="shared" ref="F93:H93" si="46">AVERAGE(F83:F92)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G93" t="e">
+      <c r="B102" t="e">
+        <f t="shared" ref="B102" si="43">AVERAGE(B92:B101)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C102" t="e">
+        <f t="shared" ref="C102" si="44">AVERAGE(C92:C101)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D102" t="e">
+        <f t="shared" ref="D102" si="45">AVERAGE(D92:D101)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F102" t="e">
+        <f t="shared" ref="F102:H102" si="46">AVERAGE(F92:F101)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G102" t="e">
         <f t="shared" si="46"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H93" t="e">
+      <c r="H102" t="e">
         <f t="shared" si="46"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J93" t="e">
-        <f t="shared" ref="J93:L93" si="47">AVERAGE(J83:J92)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K93" t="e">
+      <c r="J102" t="e">
+        <f t="shared" ref="J102:L102" si="47">AVERAGE(J92:J101)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K102" t="e">
         <f t="shared" si="47"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="L93" t="e">
+      <c r="L102" t="e">
         <f t="shared" si="47"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="N93" t="e">
-        <f t="shared" ref="N93:P93" si="48">AVERAGE(N83:N92)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O93" t="e">
+      <c r="N102" t="e">
+        <f t="shared" ref="N102:P102" si="48">AVERAGE(N92:N101)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O102" t="e">
         <f t="shared" si="48"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="P93" t="e">
+      <c r="P102" t="e">
         <f t="shared" si="48"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="94" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
+    <row r="103" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
         <v>3</v>
       </c>
-      <c r="B94" t="e">
-        <f>STDEV(B83:B92)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C94" t="e">
-        <f>STDEV(C83:C92)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D94" t="e">
-        <f t="shared" ref="D94" si="49">STDEV(D83:D92)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F94" t="e">
-        <f>STDEV(F83:F92)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G94" t="e">
-        <f>STDEV(G83:G92)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H94" t="e">
-        <f t="shared" ref="H94" si="50">STDEV(H83:H92)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J94" t="e">
-        <f>STDEV(J83:J92)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K94" t="e">
-        <f>STDEV(K83:K92)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L94" t="e">
-        <f t="shared" ref="L94" si="51">STDEV(L83:L92)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N94" t="e">
-        <f>STDEV(N83:N92)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O94" t="e">
-        <f>STDEV(O83:O92)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P94" t="e">
-        <f t="shared" ref="P94" si="52">STDEV(P83:P92)</f>
+      <c r="B103" t="e">
+        <f>STDEV(B92:B101)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C103" t="e">
+        <f>STDEV(C92:C101)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D103" t="e">
+        <f t="shared" ref="D103" si="49">STDEV(D92:D101)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F103" t="e">
+        <f>STDEV(F92:F101)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G103" t="e">
+        <f>STDEV(G92:G101)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H103" t="e">
+        <f t="shared" ref="H103" si="50">STDEV(H92:H101)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J103" t="e">
+        <f>STDEV(J92:J101)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K103" t="e">
+        <f>STDEV(K92:K101)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L103" t="e">
+        <f t="shared" ref="L103" si="51">STDEV(L92:L101)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N103" t="e">
+        <f>STDEV(N92:N101)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O103" t="e">
+        <f>STDEV(O92:O101)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P103" t="e">
+        <f t="shared" ref="P103" si="52">STDEV(P92:P101)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="25">
-    <mergeCell ref="N81:P81"/>
+  <mergeCells count="33">
+    <mergeCell ref="N90:P90"/>
+    <mergeCell ref="B32:C34"/>
+    <mergeCell ref="D32:D34"/>
+    <mergeCell ref="B36:C38"/>
+    <mergeCell ref="D36:D38"/>
+    <mergeCell ref="F32:G34"/>
+    <mergeCell ref="H32:H34"/>
+    <mergeCell ref="F36:G38"/>
+    <mergeCell ref="H36:H38"/>
     <mergeCell ref="N6:P6"/>
     <mergeCell ref="N17:P17"/>
-    <mergeCell ref="N33:P33"/>
-    <mergeCell ref="N49:P49"/>
-    <mergeCell ref="N65:P65"/>
+    <mergeCell ref="N42:P42"/>
+    <mergeCell ref="N58:P58"/>
+    <mergeCell ref="N74:P74"/>
     <mergeCell ref="J17:L17"/>
-    <mergeCell ref="J33:L33"/>
-    <mergeCell ref="J49:L49"/>
-    <mergeCell ref="J65:L65"/>
-    <mergeCell ref="J81:L81"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="B49:D49"/>
-    <mergeCell ref="B65:D65"/>
-    <mergeCell ref="B81:D81"/>
+    <mergeCell ref="J42:L42"/>
+    <mergeCell ref="J58:L58"/>
+    <mergeCell ref="J74:L74"/>
+    <mergeCell ref="J90:L90"/>
+    <mergeCell ref="B42:D42"/>
+    <mergeCell ref="B58:D58"/>
+    <mergeCell ref="B74:D74"/>
+    <mergeCell ref="B90:D90"/>
     <mergeCell ref="F6:H6"/>
     <mergeCell ref="F17:H17"/>
-    <mergeCell ref="F33:H33"/>
-    <mergeCell ref="F49:H49"/>
-    <mergeCell ref="F65:H65"/>
-    <mergeCell ref="F81:H81"/>
+    <mergeCell ref="F42:H42"/>
+    <mergeCell ref="F58:H58"/>
+    <mergeCell ref="F74:H74"/>
+    <mergeCell ref="F90:H90"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="B6:D6"/>
     <mergeCell ref="B17:D17"/>

</xml_diff>